<commit_message>
Complete Docker removal - no Docker anywhere in codebase
</commit_message>
<xml_diff>
--- a/teacher_import_template.xlsx
+++ b/teacher_import_template.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Teachers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,40 +447,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>phone_number</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>phone_number</t>
+          <t>subjects</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>subjects</t>
+          <t>classes_assigned</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>classes_assigned</t>
+          <t>qualification</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>qualification</t>
+          <t>experience_years</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>experience_years</t>
+          <t>address</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>address</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>emergency_contact</t>
         </is>
@@ -493,95 +489,350 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Patel</t>
+          <t>Sharma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>priya.patel@school.com</t>
+          <t>9876601001</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9876543210</t>
+          <t>Mathematics,Science</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mathematics,Science</t>
+          <t>Class 7,Class 8</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>7,8</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>M.Sc Mathematics</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>5</v>
+      <c r="G2" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15 Koramangala, Bangalore</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>123 Teacher Colony</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>9876543212</t>
+          <t>9876602001</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Amit</t>
+          <t>Ravi</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Singh</t>
+          <t>Verma</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>amit.singh@school.com</t>
+          <t>9876601002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9876543211</t>
+          <t>English,Hindi</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>English,Hindi</t>
+          <t>Class 9,Class 10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>9,10</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>M.A English</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>8</v>
+          <t>M.A English Literature</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>32 Banjara Hills, Hyderabad</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>456 Staff Quarters</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>9876543213</t>
+          <t>9876602002</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Meena</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nair</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9876601003</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Social Studies,History</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Class 7,Class 9</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>M.A History</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>67 Andheri West, Mumbai</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>9876602003</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Suresh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Patel</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>9876601004</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Physics,Chemistry</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Class 8,Class 10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>M.Sc Physics</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>89 Satellite, Ahmedabad</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>9876602004</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kavita</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Joshi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>9876601005</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Biology,Mathematics</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Class 7,Class 8</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>M.Sc Zoology</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>44 Sadashiv Peth, Pune</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>9876602005</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1. Fill in teacher details in the Teachers sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2. Required fields: first_name, last_name, phone_number</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3. Phone numbers: 10 digits (e.g., 9876543210)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4. Subjects: Comma-separated (e.g., "Mathematics,Science")</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5. Classes: Comma-separated (e.g., "Class 7,Class 8")</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6. Phone number must be unique</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7. Email is auto-generated from phone number</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8. Upload this file in Admin Panel -&gt; Import Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Note: This template has 5 sample teachers ready to import!</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Login Credentials:</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>- Teachers log in via mobile app using OTP</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>- Use the phone number from the import</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>- No password needed for mobile login</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>- OTP will be sent to the phone number</t>
         </is>
       </c>
     </row>

</xml_diff>